<commit_message>
Adding performance review folder to repo
</commit_message>
<xml_diff>
--- a/annualreviews.xlsx
+++ b/annualreviews.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gjames\Desktop\HR_BHN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12EE8F87-5199-43BB-9803-5E0B56EE8C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE818B62-8E05-4F20-BA76-66887654777C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A2FB4637-7180-48EA-A534-AF23FA68B170}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A2FB4637-7180-48EA-A534-AF23FA68B170}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
   <si>
     <t>SupervisorName</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Wendy Orson</t>
   </si>
   <si>
-    <t>worson@bhnstl.org</t>
-  </si>
-  <si>
     <t>Elizabeth Gebhart</t>
   </si>
   <si>
@@ -77,15 +74,9 @@
     <t>Holly Campbell</t>
   </si>
   <si>
-    <t>jmiller@bhnstl.org</t>
-  </si>
-  <si>
     <t>Kayla Dairaghi</t>
   </si>
   <si>
-    <t>bwing@bhnstl.org</t>
-  </si>
-  <si>
     <t>Fred Evans</t>
   </si>
   <si>
@@ -95,21 +86,12 @@
     <t>Tamela Wright</t>
   </si>
   <si>
-    <t>twright@bhnstl.org</t>
-  </si>
-  <si>
     <t>Chris Hotard</t>
   </si>
   <si>
-    <t>dsilverblatt@bhnstl.org</t>
-  </si>
-  <si>
     <t>Gabby James</t>
   </si>
   <si>
-    <t>egebhart@bhnstl.org</t>
-  </si>
-  <si>
     <t>Shalese Johnson</t>
   </si>
   <si>
@@ -131,10 +113,10 @@
     <t>Nicole Wood</t>
   </si>
   <si>
-    <t>mchilds@bhnstl.org</t>
-  </si>
-  <si>
     <t>Jackie Hawkins</t>
+  </si>
+  <si>
+    <t>gjames@bhnstl.org</t>
   </si>
 </sst>
 </file>
@@ -530,7 +512,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -567,7 +549,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2">
         <v>45112</v>
@@ -578,13 +560,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D3" s="2">
         <v>44872</v>
@@ -595,13 +577,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2">
         <v>45012</v>
@@ -612,13 +594,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2">
         <v>43626</v>
@@ -629,13 +611,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2">
         <v>44109</v>
@@ -646,13 +628,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2">
         <v>45082</v>
@@ -663,13 +645,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D8" s="2">
         <v>43735</v>
@@ -680,13 +662,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D9" s="2">
         <v>44810</v>
@@ -697,13 +679,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D10" s="2">
         <v>45293</v>
@@ -714,13 +696,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D11" s="2">
         <v>44536</v>
@@ -731,13 +713,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D12" s="2">
         <v>44872</v>
@@ -748,13 +730,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D13" s="2">
         <v>45222</v>
@@ -765,13 +747,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D14" s="2">
         <v>42226</v>
@@ -782,13 +764,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D15" s="2">
         <v>44747</v>
@@ -799,13 +781,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D16" s="2">
         <v>44788</v>
@@ -816,13 +798,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D17" s="2">
         <v>43983</v>
@@ -833,13 +815,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D18" s="2">
         <v>45038</v>
@@ -850,13 +832,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D19" s="2">
         <v>44648</v>
@@ -867,13 +849,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D20" s="2">
         <v>42738</v>
@@ -884,13 +866,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D21" s="2">
         <v>45460</v>
@@ -902,25 +884,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{5D7C5DED-7300-41D8-B0E9-7F827B3541F5}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{CD5A34D1-BF31-42EC-A071-A9E3BBF66406}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{C571FCF7-71ED-4A10-AE06-E8D0C17C02FD}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{D8EB7C77-27D0-47C0-B4E5-C81FFDA5C0BC}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{1C2DF6E6-653F-4AC6-B24E-B9B5CF1C3922}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{F0EB78CB-6CD2-4B94-927A-EFED2AEACE6F}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{31F1F85C-FA58-46C3-A42F-0D181F4BBA8C}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{C1DF38A8-38BE-4F79-A137-4F2668B2E3D8}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{AF7489E7-68A2-46B9-BF65-8D19F1BBA446}"/>
-    <hyperlink ref="C11" r:id="rId10" xr:uid="{D317AC22-6CFB-44E8-A129-DC716DDCE9EB}"/>
-    <hyperlink ref="C12" r:id="rId11" xr:uid="{D7F270DB-2009-4499-9630-75360786E069}"/>
-    <hyperlink ref="C13" r:id="rId12" xr:uid="{E221C4F4-C26C-4997-8550-8A86AE6C43CC}"/>
-    <hyperlink ref="C14" r:id="rId13" xr:uid="{18129CAB-910C-40E3-83E8-FAB82D3BB804}"/>
-    <hyperlink ref="C15" r:id="rId14" xr:uid="{1E2BD630-1E89-4DDD-8F09-0E31E5E97641}"/>
-    <hyperlink ref="C16" r:id="rId15" xr:uid="{BF7594BA-714F-4DA3-9465-9F48A4304631}"/>
-    <hyperlink ref="C17" r:id="rId16" xr:uid="{F5711BB5-D47E-4F8A-80D0-91B16DF6D184}"/>
-    <hyperlink ref="C18" r:id="rId17" xr:uid="{E6C70CBD-65BE-47C7-8F74-88AAFC8F8D07}"/>
-    <hyperlink ref="C19" r:id="rId18" xr:uid="{92EAA6EC-961D-4702-8D47-00C814C84902}"/>
-    <hyperlink ref="C20" r:id="rId19" xr:uid="{F81C9A5E-4B84-4F9E-87FE-69B5D5DE3415}"/>
-    <hyperlink ref="C21" r:id="rId20" xr:uid="{18460486-DFE7-4802-880A-A9A9BE52A07D}"/>
+    <hyperlink ref="C3:C21" r:id="rId2" display="gjames@bhnstl.org" xr:uid="{C964B7A8-BEB0-46A2-9684-6C79D22F1E02}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>